<commit_message>
new field added in spare details
</commit_message>
<xml_diff>
--- a/Presentation/Casa.API/FormatFiles/Template_SpareDetails.xlsx
+++ b/Presentation/Casa.API/FormatFiles/Template_SpareDetails.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PartCode</t>
   </si>
@@ -37,18 +37,9 @@
     <t>KG</t>
   </si>
   <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>MTS</t>
-  </si>
-  <si>
     <t>SpareCategory</t>
   </si>
   <si>
-    <t>Cell</t>
-  </si>
-  <si>
     <t>Consumable</t>
   </si>
   <si>
@@ -59,6 +50,18 @@
   </si>
   <si>
     <t>TentativeCost</t>
+  </si>
+  <si>
+    <t>ProductMake</t>
+  </si>
+  <si>
+    <t>BMSMake</t>
+  </si>
+  <si>
+    <t>FBTECH</t>
+  </si>
+  <si>
+    <t>Udaan</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -423,11 +426,13 @@
     <col min="4" max="5" width="9.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="12" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -442,21 +447,27 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>123</v>
@@ -476,45 +487,22 @@
       <c r="G2" s="2">
         <v>10.210000000000001</v>
       </c>
-      <c r="H2" t="b">
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" t="b">
+      <c r="K2" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2">
-        <v>10</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I3 H2:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K2 J2:J1048576">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
issue fixed and added region and state in branch api
</commit_message>
<xml_diff>
--- a/Presentation/Casa.API/FormatFiles/Template_SpareDetails.xlsx
+++ b/Presentation/Casa.API/FormatFiles/Template_SpareDetails.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>PartCode</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>UOM</t>
   </si>
@@ -55,13 +49,13 @@
     <t>ProductMake</t>
   </si>
   <si>
-    <t>BMSMake</t>
-  </si>
-  <si>
     <t>FBTECH</t>
   </si>
   <si>
-    <t>Udaan</t>
+    <t>SparePartCode</t>
+  </si>
+  <si>
+    <t>SparePartDescription</t>
   </si>
 </sst>
 </file>
@@ -412,97 +406,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="5" width="9.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="G2" s="2">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="H2" s="2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K2 J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J2 I2:I1048576">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>